<commit_message>
Updated README with more information
</commit_message>
<xml_diff>
--- a/data-formatter.xlsx
+++ b/data-formatter.xlsx
@@ -661,10 +661,10 @@
   <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="12.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.22"/>
@@ -718,8 +718,8 @@
         <v>04/08/24</v>
       </c>
       <c r="B2" s="4" t="str">
-        <f aca="false">raw!E2</f>
-        <v>9:00 PM</v>
+        <f aca="false">"0"&amp;raw!E2</f>
+        <v>09:00 PM</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>11</v>
@@ -757,8 +757,8 @@
         <v>04/08/24</v>
       </c>
       <c r="B3" s="8" t="str">
-        <f aca="false">raw!E3</f>
-        <v>8:00 PM</v>
+        <f aca="false">"0"&amp;raw!E3</f>
+        <v>08:00 PM</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>11</v>
@@ -796,8 +796,8 @@
         <v>04/13/24</v>
       </c>
       <c r="B4" s="4" t="str">
-        <f aca="false">raw!E4</f>
-        <v>2:00 PM</v>
+        <f aca="false">"0"&amp;raw!E4</f>
+        <v>02:00 PM</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>11</v>
@@ -835,8 +835,8 @@
         <v>04/13/24</v>
       </c>
       <c r="B5" s="8" t="str">
-        <f aca="false">raw!E5</f>
-        <v>3:00 PM</v>
+        <f aca="false">"0"&amp;raw!E5</f>
+        <v>03:00 PM</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>11</v>
@@ -868,8 +868,8 @@
         <v>04/16/24</v>
       </c>
       <c r="B6" s="4" t="str">
-        <f aca="false">raw!E6</f>
-        <v>8:00 PM</v>
+        <f aca="false">"0"&amp;raw!E6</f>
+        <v>08:00 PM</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>11</v>
@@ -901,8 +901,8 @@
         <v>04/16/24</v>
       </c>
       <c r="B7" s="8" t="str">
-        <f aca="false">raw!E7</f>
-        <v>9:00 PM</v>
+        <f aca="false">"0"&amp;raw!E7</f>
+        <v>09:00 PM</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>11</v>
@@ -934,8 +934,8 @@
         <v>05/02/24</v>
       </c>
       <c r="B8" s="4" t="str">
-        <f aca="false">raw!E8</f>
-        <v>6:00 PM</v>
+        <f aca="false">"0"&amp;raw!E8</f>
+        <v>06:00 PM</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>11</v>
@@ -967,8 +967,8 @@
         <v>05/02/24</v>
       </c>
       <c r="B9" s="8" t="str">
-        <f aca="false">raw!E9</f>
-        <v>7:00 PM</v>
+        <f aca="false">"0"&amp;raw!E9</f>
+        <v>07:00 PM</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>11</v>
@@ -1000,8 +1000,8 @@
         <v>05/06/24</v>
       </c>
       <c r="B10" s="4" t="str">
-        <f aca="false">raw!E10</f>
-        <v>8:00 PM</v>
+        <f aca="false">"0"&amp;raw!E10</f>
+        <v>08:00 PM</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>11</v>
@@ -1033,8 +1033,8 @@
         <v>05/06/24</v>
       </c>
       <c r="B11" s="8" t="str">
-        <f aca="false">raw!E11</f>
-        <v>9:00 PM</v>
+        <f aca="false">"0"&amp;raw!E11</f>
+        <v>09:00 PM</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>11</v>
@@ -1066,8 +1066,8 @@
         <v>05/22/24</v>
       </c>
       <c r="B12" s="4" t="str">
-        <f aca="false">raw!E12</f>
-        <v>6:00 PM</v>
+        <f aca="false">"0"&amp;raw!E12</f>
+        <v>06:00 PM</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>11</v>
@@ -1099,8 +1099,8 @@
         <v>05/22/24</v>
       </c>
       <c r="B13" s="8" t="str">
-        <f aca="false">raw!E13</f>
-        <v>7:00 PM</v>
+        <f aca="false">"0"&amp;raw!E13</f>
+        <v>07:00 PM</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>11</v>
@@ -1132,8 +1132,8 @@
         <v>05/28/24</v>
       </c>
       <c r="B14" s="4" t="str">
-        <f aca="false">raw!E14</f>
-        <v>8:00 PM</v>
+        <f aca="false">"0"&amp;raw!E14</f>
+        <v>08:00 PM</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>11</v>
@@ -1165,8 +1165,8 @@
         <v>05/28/24</v>
       </c>
       <c r="B15" s="8" t="str">
-        <f aca="false">raw!E15</f>
-        <v>9:00 PM</v>
+        <f aca="false">"0"&amp;raw!E15</f>
+        <v>09:00 PM</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>11</v>
@@ -1198,8 +1198,8 @@
         <v>06/03/24</v>
       </c>
       <c r="B16" s="4" t="str">
-        <f aca="false">raw!E16</f>
-        <v>6:00 PM</v>
+        <f aca="false">"0"&amp;raw!E16</f>
+        <v>06:00 PM</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>11</v>
@@ -1231,8 +1231,8 @@
         <v>06/03/24</v>
       </c>
       <c r="B17" s="8" t="str">
-        <f aca="false">raw!E17</f>
-        <v>7:00 PM</v>
+        <f aca="false">"0"&amp;raw!E17</f>
+        <v>07:00 PM</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>11</v>
@@ -1264,8 +1264,8 @@
         <v>06/04/24</v>
       </c>
       <c r="B18" s="4" t="str">
-        <f aca="false">raw!E18</f>
-        <v>6:00 PM</v>
+        <f aca="false">"0"&amp;raw!E18</f>
+        <v>06:00 PM</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>11</v>
@@ -1297,8 +1297,8 @@
         <v>06/04/24</v>
       </c>
       <c r="B19" s="8" t="str">
-        <f aca="false">raw!E19</f>
-        <v>7:00 PM</v>
+        <f aca="false">"0"&amp;raw!E19</f>
+        <v>07:00 PM</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>11</v>
@@ -1330,8 +1330,8 @@
         <v>06/11/24</v>
       </c>
       <c r="B20" s="4" t="str">
-        <f aca="false">raw!E20</f>
-        <v>6:00 PM</v>
+        <f aca="false">"0"&amp;raw!E20</f>
+        <v>06:00 PM</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>11</v>
@@ -1363,8 +1363,8 @@
         <v>06/11/24</v>
       </c>
       <c r="B21" s="8" t="str">
-        <f aca="false">raw!E21</f>
-        <v>7:00 PM</v>
+        <f aca="false">"0"&amp;raw!E21</f>
+        <v>07:00 PM</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>11</v>
@@ -1396,8 +1396,8 @@
         <v>06/13/24</v>
       </c>
       <c r="B22" s="4" t="str">
-        <f aca="false">raw!E22</f>
-        <v>8:00 PM</v>
+        <f aca="false">"0"&amp;raw!E22</f>
+        <v>08:00 PM</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>11</v>
@@ -1429,8 +1429,8 @@
         <v>06/13/24</v>
       </c>
       <c r="B23" s="8" t="str">
-        <f aca="false">raw!E23</f>
-        <v>9:00 PM</v>
+        <f aca="false">"0"&amp;raw!E23</f>
+        <v>09:00 PM</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>11</v>
@@ -1704,7 +1704,7 @@
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
@@ -2414,7 +2414,7 @@
       <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="19" t="s">

</xml_diff>